<commit_message>
Update TestDBSchemeForFMS.xlsx (Add "total" field to the "invoice" table)
</commit_message>
<xml_diff>
--- a/dist-docs/TestDBSchemeForFMS.xlsx
+++ b/dist-docs/TestDBSchemeForFMS.xlsx
@@ -45,118 +45,37 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="134">
-  <si>
-    <t>user_id</t>
-  </si>
-  <si>
-    <t>group_id</t>
-  </si>
-  <si>
-    <t>dest_group_id</t>
-  </si>
-  <si>
-    <t>privname</t>
-  </si>
-  <si>
-    <t>clienthost</t>
-  </si>
-  <si>
-    <t>hash</t>
-  </si>
-  <si>
-    <t>expired</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="137">
+  <si>
+    <t>registereddt</t>
+  </si>
+  <si>
+    <t>テキスト</t>
+    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>タイムスタンプ</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>num1</t>
-  </si>
-  <si>
-    <t>num2</t>
-  </si>
-  <si>
-    <t>num3</t>
-  </si>
-  <si>
-    <t>dt1</t>
-  </si>
-  <si>
-    <t>dt2</t>
-  </si>
-  <si>
-    <t>dt3</t>
-  </si>
-  <si>
-    <t>vc1</t>
-  </si>
-  <si>
-    <t>vc2</t>
-  </si>
-  <si>
-    <t>vc3</t>
-  </si>
-  <si>
-    <t>text1</t>
-  </si>
-  <si>
-    <t>text2</t>
-  </si>
-  <si>
-    <t>タイムスタンプ</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>タイムスタンプ</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>タイムスタンプ</t>
-    <phoneticPr fontId="1"/>
+    <t>context_id</t>
+  </si>
+  <si>
+    <t>pk</t>
+  </si>
+  <si>
+    <t>hashedpasswd</t>
+  </si>
+  <si>
+    <t>email</t>
   </si>
   <si>
     <t>テキスト</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>テキスト</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>テキスト</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>テキスト</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>dt</t>
-  </si>
-  <si>
-    <t>item</t>
-  </si>
-  <si>
-    <t>customer</t>
-  </si>
-  <si>
-    <t>item_id</t>
-  </si>
-  <si>
-    <t>customer_id</t>
-  </si>
-  <si>
-    <t>タイムスタンプ</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>total</t>
     <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>unitprice_master</t>
   </si>
   <si>
     <t>計算</t>
@@ -166,6 +85,128 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>Sum ( item::amount )</t>
+  </si>
+  <si>
+    <t>user_id</t>
+  </si>
+  <si>
+    <t>group_id</t>
+  </si>
+  <si>
+    <t>dest_group_id</t>
+  </si>
+  <si>
+    <t>privname</t>
+  </si>
+  <si>
+    <t>clienthost</t>
+  </si>
+  <si>
+    <t>hash</t>
+  </si>
+  <si>
+    <t>expired</t>
+  </si>
+  <si>
+    <t>タイムスタンプ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>num1</t>
+  </si>
+  <si>
+    <t>num2</t>
+  </si>
+  <si>
+    <t>num3</t>
+  </si>
+  <si>
+    <t>dt1</t>
+  </si>
+  <si>
+    <t>dt2</t>
+  </si>
+  <si>
+    <t>dt3</t>
+  </si>
+  <si>
+    <t>vc1</t>
+  </si>
+  <si>
+    <t>vc2</t>
+  </si>
+  <si>
+    <t>vc3</t>
+  </si>
+  <si>
+    <t>text1</t>
+  </si>
+  <si>
+    <t>text2</t>
+  </si>
+  <si>
+    <t>タイムスタンプ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>タイムスタンプ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>タイムスタンプ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>テキスト</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>テキスト</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>テキスト</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>テキスト</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>dt</t>
+  </si>
+  <si>
+    <t>item</t>
+  </si>
+  <si>
+    <t>customer</t>
+  </si>
+  <si>
+    <t>item_id</t>
+  </si>
+  <si>
+    <t>customer_id</t>
+  </si>
+  <si>
+    <t>タイムスタンプ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>total</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>unitprice_master</t>
+  </si>
+  <si>
+    <t>計算</t>
+    <rPh sb="0" eb="2">
+      <t>ケイサン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>qty * If( unitprice = ""; product::unitprice; unitprice )</t>
   </si>
   <si>
@@ -478,33 +519,6 @@
   </si>
   <si>
     <t>conditions</t>
-  </si>
-  <si>
-    <t>registereddt</t>
-  </si>
-  <si>
-    <t>テキスト</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>タイムスタンプ</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>context_id</t>
-  </si>
-  <si>
-    <t>pk</t>
-  </si>
-  <si>
-    <t>hashedpasswd</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>テキスト</t>
-    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
@@ -913,75 +927,75 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" ht="19">
       <c r="A5" s="2" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>54</v>
+        <v>65</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" ht="19">
       <c r="A6" s="2" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" ht="19">
       <c r="A7" s="2" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" ht="19">
       <c r="A8" s="2" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="C8" s="1"/>
     </row>
@@ -1012,84 +1026,84 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="3" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="4" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C2" s="3"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="4" t="s">
-        <v>89</v>
+        <v>100</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C3" s="3"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="4" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C4" s="3"/>
     </row>
     <row r="5" spans="1:3" ht="19">
       <c r="A5" s="4" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="C5" s="3"/>
     </row>
     <row r="6" spans="1:3" ht="19">
       <c r="A6" s="4" t="s">
-        <v>93</v>
+        <v>104</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>96</v>
+        <v>107</v>
       </c>
       <c r="C6" s="3"/>
     </row>
     <row r="7" spans="1:3" ht="19">
       <c r="A7" s="4" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="C7" s="3"/>
     </row>
     <row r="8" spans="1:3" ht="19">
       <c r="A8" s="4" t="s">
-        <v>95</v>
+        <v>106</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>97</v>
+        <v>108</v>
       </c>
       <c r="C8" s="3"/>
     </row>
     <row r="9" spans="1:3" ht="19">
       <c r="A9" s="4" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="C9" s="3"/>
     </row>
@@ -1120,84 +1134,84 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>98</v>
+        <v>109</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" ht="19">
       <c r="A5" s="2" t="s">
-        <v>99</v>
+        <v>110</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" ht="19">
       <c r="A6" s="2" t="s">
-        <v>100</v>
+        <v>111</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" ht="19">
       <c r="A7" s="2" t="s">
-        <v>101</v>
+        <v>112</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" ht="19">
       <c r="A8" s="2" t="s">
-        <v>102</v>
+        <v>113</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:3" ht="19">
       <c r="A9" s="2" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="C9" s="1"/>
     </row>
@@ -1228,66 +1242,66 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>103</v>
+        <v>114</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>98</v>
+        <v>109</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>104</v>
+        <v>115</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" ht="19">
       <c r="A5" s="2" t="s">
-        <v>105</v>
+        <v>116</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" ht="19">
       <c r="A6" s="2" t="s">
-        <v>106</v>
+        <v>117</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" ht="19">
       <c r="A7" s="2" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="C7" s="1"/>
     </row>
@@ -1328,48 +1342,48 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>104</v>
+        <v>115</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>108</v>
+        <v>119</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" ht="19">
       <c r="A5" s="2" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="C5" s="1"/>
     </row>
@@ -1420,30 +1434,30 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>89</v>
+        <v>100</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="C3" s="1"/>
     </row>
@@ -1504,57 +1518,57 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>110</v>
+        <v>121</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>96</v>
+        <v>107</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" ht="19">
       <c r="A5" s="2" t="s">
-        <v>111</v>
+        <v>122</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>114</v>
+        <v>125</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" ht="19">
       <c r="A6" s="2" t="s">
-        <v>112</v>
+        <v>123</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="C6" s="1"/>
     </row>
@@ -1600,39 +1614,39 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>116</v>
+        <v>127</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>117</v>
+        <v>128</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="C4" s="1"/>
     </row>
@@ -1688,66 +1702,66 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>118</v>
+        <v>129</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>119</v>
+        <v>130</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" ht="19">
       <c r="A5" s="2" t="s">
-        <v>120</v>
+        <v>131</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" ht="19">
       <c r="A6" s="2" t="s">
-        <v>121</v>
+        <v>132</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" ht="19">
       <c r="A7" s="2" t="s">
-        <v>122</v>
+        <v>133</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="C7" s="1"/>
     </row>
@@ -1788,57 +1802,57 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>123</v>
+        <v>134</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>127</v>
+        <v>1</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" ht="19">
       <c r="A5" s="2" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" ht="19">
       <c r="A6" s="2" t="s">
-        <v>126</v>
+        <v>0</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>128</v>
+        <v>2</v>
       </c>
       <c r="C6" s="1"/>
     </row>
@@ -1884,30 +1898,30 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>129</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>130</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C3" s="1"/>
     </row>
@@ -1968,84 +1982,84 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>62</v>
+        <v>73</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" ht="19">
       <c r="A5" s="2" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" ht="19">
       <c r="A6" s="2" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" ht="19">
       <c r="A7" s="2" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" ht="19">
       <c r="A8" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>49</v>
       </c>
       <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:3" ht="19">
       <c r="A9" s="2" t="s">
-        <v>61</v>
+        <v>72</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C9" s="1"/>
     </row>
@@ -2076,48 +2090,48 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>131</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" ht="19">
       <c r="A5" s="2" t="s">
-        <v>132</v>
+        <v>6</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>133</v>
+        <v>7</v>
       </c>
       <c r="C5" s="1"/>
     </row>
@@ -2168,30 +2182,30 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>110</v>
+        <v>121</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>96</v>
+        <v>107</v>
       </c>
       <c r="C3" s="1"/>
     </row>
@@ -2252,57 +2266,57 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" ht="19">
       <c r="A5" s="2" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" ht="19">
       <c r="A6" s="2" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>127</v>
+        <v>1</v>
       </c>
       <c r="C6" s="1"/>
     </row>
@@ -2348,57 +2362,57 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" ht="19">
       <c r="A5" s="2" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" ht="19">
       <c r="A6" s="2" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="C6" s="1"/>
     </row>
@@ -2444,120 +2458,120 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" ht="19">
       <c r="A5" s="2" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" ht="19">
       <c r="A6" s="2" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" ht="19">
       <c r="A7" s="2" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" ht="19">
       <c r="A8" s="2" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:3" ht="19">
       <c r="A9" s="2" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:3" ht="19">
       <c r="A10" s="2" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:3" ht="19">
       <c r="A11" s="2" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="C11" s="1"/>
     </row>
     <row r="12" spans="1:3" ht="19">
       <c r="A12" s="2" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="C12" s="1"/>
     </row>
     <row r="13" spans="1:3" ht="19">
       <c r="A13" s="2" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="C13" s="1"/>
     </row>
@@ -2588,93 +2602,93 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" ht="19">
       <c r="A5" s="2" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" ht="19">
       <c r="A6" s="2" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" ht="19">
       <c r="A7" s="2" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" ht="19">
       <c r="A8" s="2" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:3" ht="19">
       <c r="A9" s="2" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:3" ht="19">
       <c r="A10" s="2" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C10" s="1"/>
     </row>
@@ -2720,39 +2734,39 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C4" s="1"/>
     </row>
@@ -2828,30 +2842,30 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>113</v>
+        <v>124</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="C3" s="1"/>
     </row>
@@ -2932,30 +2946,30 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="C3" s="1"/>
     </row>
@@ -3016,30 +3030,30 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>66</v>
+        <v>77</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
       <c r="C3" s="1"/>
     </row>
@@ -3100,39 +3114,39 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>68</v>
+        <v>79</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C4" s="1"/>
     </row>
@@ -3188,66 +3202,66 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" ht="19">
       <c r="A5" s="2" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" ht="19">
       <c r="A6" s="2" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" ht="19">
       <c r="A7" s="2" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>75</v>
+        <v>86</v>
       </c>
       <c r="C7" s="1"/>
     </row>
@@ -3288,66 +3302,66 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" ht="19">
       <c r="A5" s="2" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" ht="19">
       <c r="A6" s="2" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" ht="19">
       <c r="A7" s="2" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="C7" s="1"/>
     </row>
@@ -3378,83 +3392,92 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView view="pageLayout" workbookViewId="0"/>
+    <sheetView view="pageLayout" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="17"/>
   <cols>
     <col min="1" max="1" width="20.83203125" customWidth="1"/>
     <col min="2" max="2" width="15.83203125" customWidth="1"/>
+    <col min="3" max="3" width="24" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>82</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>71</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>83</v>
+        <v>94</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" ht="19">
       <c r="A5" s="2" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" ht="19">
       <c r="A6" s="2" t="s">
-        <v>85</v>
+        <v>96</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" ht="19">
       <c r="A7" s="2" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" ht="19">
-      <c r="A8" s="2"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
+      <c r="A8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="9" spans="1:3" ht="19">
       <c r="A9" s="2"/>
@@ -3489,100 +3512,100 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>51</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>89</v>
+        <v>100</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" ht="19">
       <c r="A5" s="2" t="s">
-        <v>90</v>
+        <v>101</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" ht="19">
       <c r="A6" s="2" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" ht="19">
       <c r="A7" s="2" t="s">
-        <v>92</v>
+        <v>103</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" ht="19">
       <c r="A8" s="2" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="19">
       <c r="A9" s="2" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="18">
       <c r="A10" s="1" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update TestDB.fmp12 to fix portal access mode in sample application
</commit_message>
<xml_diff>
--- a/dist-docs/TestDBSchemeForFMS.xlsx
+++ b/dist-docs/TestDBSchemeForFMS.xlsx
@@ -45,7 +45,38 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="135">
+  <si>
+    <t>registereddt</t>
+  </si>
+  <si>
+    <t>テキスト</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>タイムスタンプ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>context_id</t>
+  </si>
+  <si>
+    <t>pk</t>
+  </si>
+  <si>
+    <t>hashedpasswd</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>テキスト</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>memo</t>
+    <phoneticPr fontId="1"/>
+  </si>
   <si>
     <t>user_id</t>
   </si>
@@ -478,33 +509,6 @@
   </si>
   <si>
     <t>conditions</t>
-  </si>
-  <si>
-    <t>registereddt</t>
-  </si>
-  <si>
-    <t>テキスト</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>タイムスタンプ</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>context_id</t>
-  </si>
-  <si>
-    <t>pk</t>
-  </si>
-  <si>
-    <t>hashedpasswd</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>テキスト</t>
-    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
@@ -901,7 +905,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" workbookViewId="0"/>
   </sheetViews>
@@ -913,77 +917,85 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" ht="19">
       <c r="A5" s="2" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" ht="19">
       <c r="A6" s="2" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" ht="19">
       <c r="A7" s="2" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" ht="19">
       <c r="A8" s="2" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="C8" s="1"/>
+    </row>
+    <row r="9" spans="1:3" ht="19">
+      <c r="A9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
@@ -1012,84 +1024,84 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="3" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="4" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C2" s="3"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="4" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C3" s="3"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="4" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C4" s="3"/>
     </row>
     <row r="5" spans="1:3" ht="19">
       <c r="A5" s="4" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="C5" s="3"/>
     </row>
     <row r="6" spans="1:3" ht="19">
       <c r="A6" s="4" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="C6" s="3"/>
     </row>
     <row r="7" spans="1:3" ht="19">
       <c r="A7" s="4" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="C7" s="3"/>
     </row>
     <row r="8" spans="1:3" ht="19">
       <c r="A8" s="4" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="C8" s="3"/>
     </row>
     <row r="9" spans="1:3" ht="19">
       <c r="A9" s="4" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="C9" s="3"/>
     </row>
@@ -1120,84 +1132,84 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" ht="19">
       <c r="A5" s="2" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" ht="19">
       <c r="A6" s="2" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" ht="19">
       <c r="A7" s="2" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" ht="19">
       <c r="A8" s="2" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:3" ht="19">
       <c r="A9" s="2" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="C9" s="1"/>
     </row>
@@ -1228,66 +1240,66 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" ht="19">
       <c r="A5" s="2" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" ht="19">
       <c r="A6" s="2" t="s">
-        <v>106</v>
+        <v>115</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" ht="19">
       <c r="A7" s="2" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="C7" s="1"/>
     </row>
@@ -1328,48 +1340,48 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" ht="19">
       <c r="A5" s="2" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="C5" s="1"/>
     </row>
@@ -1420,30 +1432,30 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="C3" s="1"/>
     </row>
@@ -1504,57 +1516,57 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" ht="19">
       <c r="A5" s="2" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" ht="19">
       <c r="A6" s="2" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="C6" s="1"/>
     </row>
@@ -1600,39 +1612,39 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="C4" s="1"/>
     </row>
@@ -1688,66 +1700,66 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" ht="19">
       <c r="A5" s="2" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" ht="19">
       <c r="A6" s="2" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" ht="19">
       <c r="A7" s="2" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="C7" s="1"/>
     </row>
@@ -1788,57 +1800,57 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>127</v>
+        <v>1</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" ht="19">
       <c r="A5" s="2" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" ht="19">
       <c r="A6" s="2" t="s">
-        <v>126</v>
+        <v>0</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>128</v>
+        <v>2</v>
       </c>
       <c r="C6" s="1"/>
     </row>
@@ -1884,30 +1896,30 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>129</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>130</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C3" s="1"/>
     </row>
@@ -1968,84 +1980,84 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" ht="19">
       <c r="A5" s="2" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" ht="19">
       <c r="A6" s="2" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" ht="19">
       <c r="A7" s="2" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" ht="19">
       <c r="A8" s="2" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:3" ht="19">
       <c r="A9" s="2" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C9" s="1"/>
     </row>
@@ -2076,48 +2088,48 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>131</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" ht="19">
       <c r="A5" s="2" t="s">
-        <v>132</v>
+        <v>6</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>133</v>
+        <v>7</v>
       </c>
       <c r="C5" s="1"/>
     </row>
@@ -2168,30 +2180,30 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="C3" s="1"/>
     </row>
@@ -2252,57 +2264,57 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" ht="19">
       <c r="A5" s="2" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" ht="19">
       <c r="A6" s="2" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>127</v>
+        <v>1</v>
       </c>
       <c r="C6" s="1"/>
     </row>
@@ -2348,57 +2360,57 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" ht="19">
       <c r="A5" s="2" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" ht="19">
       <c r="A6" s="2" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="C6" s="1"/>
     </row>
@@ -2444,120 +2456,120 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" ht="19">
       <c r="A5" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" ht="19">
       <c r="A6" s="2" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" ht="19">
       <c r="A7" s="2" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" ht="19">
       <c r="A8" s="2" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:3" ht="19">
       <c r="A9" s="2" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:3" ht="19">
       <c r="A10" s="2" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:3" ht="19">
       <c r="A11" s="2" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="C11" s="1"/>
     </row>
     <row r="12" spans="1:3" ht="19">
       <c r="A12" s="2" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C12" s="1"/>
     </row>
     <row r="13" spans="1:3" ht="19">
       <c r="A13" s="2" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C13" s="1"/>
     </row>
@@ -2588,93 +2600,93 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" ht="19">
       <c r="A5" s="2" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" ht="19">
       <c r="A6" s="2" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" ht="19">
       <c r="A7" s="2" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" ht="19">
       <c r="A8" s="2" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:3" ht="19">
       <c r="A9" s="2" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:3" ht="19">
       <c r="A10" s="2" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C10" s="1"/>
     </row>
@@ -2720,39 +2732,39 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C4" s="1"/>
     </row>
@@ -2828,30 +2840,30 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="C3" s="1"/>
     </row>
@@ -2932,30 +2944,30 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="C3" s="1"/>
     </row>
@@ -3016,30 +3028,30 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="C3" s="1"/>
     </row>
@@ -3100,39 +3112,39 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C4" s="1"/>
     </row>
@@ -3188,66 +3200,66 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" ht="19">
       <c r="A5" s="2" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" ht="19">
       <c r="A6" s="2" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" ht="19">
       <c r="A7" s="2" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="C7" s="1"/>
     </row>
@@ -3288,66 +3300,66 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" ht="19">
       <c r="A5" s="2" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" ht="19">
       <c r="A6" s="2" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" ht="19">
       <c r="A7" s="2" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>52</v>
+        <v>61</v>
       </c>
       <c r="C7" s="1"/>
     </row>
@@ -3388,66 +3400,66 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" ht="19">
       <c r="A5" s="2" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" ht="19">
       <c r="A6" s="2" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" ht="19">
       <c r="A7" s="2" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="C7" s="1"/>
     </row>
@@ -3489,100 +3501,100 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>51</v>
+        <v>60</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" ht="19">
       <c r="A5" s="2" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" ht="19">
       <c r="A6" s="2" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" ht="19">
       <c r="A7" s="2" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" ht="19">
       <c r="A8" s="2" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="19">
       <c r="A9" s="2" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="18">
       <c r="A10" s="1" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update TestDB.fmp12, TestDB_clone.fmp12 and TestDB.fp7 to add 'realname' field and 'limitdt' field to 'authuser' table
</commit_message>
<xml_diff>
--- a/dist-docs/TestDBSchemeForFMS.xlsx
+++ b/dist-docs/TestDBSchemeForFMS.xlsx
@@ -45,7 +45,57 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="137">
+  <si>
+    <t>タイムスタンプ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>テキスト</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>f_id</t>
+  </si>
+  <si>
+    <t>path</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>Q2</t>
+  </si>
+  <si>
+    <t>Q3</t>
+  </si>
+  <si>
+    <t>Q4</t>
+  </si>
+  <si>
+    <t>Q5</t>
+  </si>
+  <si>
+    <t>clientid</t>
+  </si>
+  <si>
+    <t>entity</t>
+  </si>
+  <si>
+    <t>conditions</t>
+  </si>
+  <si>
+    <t>realname</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>タイムスタンプ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>limitdt</t>
+    <phoneticPr fontId="1"/>
+  </si>
   <si>
     <t>registereddt</t>
   </si>
@@ -68,10 +118,6 @@
   </si>
   <si>
     <t>email</t>
-  </si>
-  <si>
-    <t>テキスト</t>
-    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>memo</t>
@@ -471,44 +517,6 @@
   <si>
     <t>id</t>
     <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>タイムスタンプ</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>テキスト</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>f_id</t>
-  </si>
-  <si>
-    <t>path</t>
-  </si>
-  <si>
-    <t>Q1</t>
-  </si>
-  <si>
-    <t>Q2</t>
-  </si>
-  <si>
-    <t>Q3</t>
-  </si>
-  <si>
-    <t>Q4</t>
-  </si>
-  <si>
-    <t>Q5</t>
-  </si>
-  <si>
-    <t>clientid</t>
-  </si>
-  <si>
-    <t>entity</t>
-  </si>
-  <si>
-    <t>conditions</t>
   </si>
 </sst>
 </file>
@@ -917,84 +925,84 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" ht="19">
       <c r="A5" s="2" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>63</v>
+        <v>77</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" ht="19">
       <c r="A6" s="2" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" ht="19">
       <c r="A7" s="2" t="s">
-        <v>54</v>
+        <v>68</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" ht="19">
       <c r="A8" s="2" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:3" ht="19">
       <c r="A9" s="2" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1024,84 +1032,84 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="3" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="4" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="C2" s="3"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="4" t="s">
-        <v>98</v>
+        <v>112</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="C3" s="3"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="4" t="s">
-        <v>101</v>
+        <v>115</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="C4" s="3"/>
     </row>
     <row r="5" spans="1:3" ht="19">
       <c r="A5" s="4" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="C5" s="3"/>
     </row>
     <row r="6" spans="1:3" ht="19">
       <c r="A6" s="4" t="s">
-        <v>102</v>
+        <v>116</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>105</v>
+        <v>119</v>
       </c>
       <c r="C6" s="3"/>
     </row>
     <row r="7" spans="1:3" ht="19">
       <c r="A7" s="4" t="s">
-        <v>103</v>
+        <v>117</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>87</v>
+        <v>101</v>
       </c>
       <c r="C7" s="3"/>
     </row>
     <row r="8" spans="1:3" ht="19">
       <c r="A8" s="4" t="s">
-        <v>104</v>
+        <v>118</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>106</v>
+        <v>120</v>
       </c>
       <c r="C8" s="3"/>
     </row>
     <row r="9" spans="1:3" ht="19">
       <c r="A9" s="4" t="s">
-        <v>90</v>
+        <v>104</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="C9" s="3"/>
     </row>
@@ -1132,84 +1140,84 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>107</v>
+        <v>121</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" ht="19">
       <c r="A5" s="2" t="s">
-        <v>108</v>
+        <v>122</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" ht="19">
       <c r="A6" s="2" t="s">
-        <v>109</v>
+        <v>123</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" ht="19">
       <c r="A7" s="2" t="s">
-        <v>110</v>
+        <v>124</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" ht="19">
       <c r="A8" s="2" t="s">
-        <v>111</v>
+        <v>125</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:3" ht="19">
       <c r="A9" s="2" t="s">
-        <v>90</v>
+        <v>104</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="C9" s="1"/>
     </row>
@@ -1240,66 +1248,66 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>112</v>
+        <v>126</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>107</v>
+        <v>121</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>113</v>
+        <v>127</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" ht="19">
       <c r="A5" s="2" t="s">
-        <v>114</v>
+        <v>128</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" ht="19">
       <c r="A6" s="2" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" ht="19">
       <c r="A7" s="2" t="s">
-        <v>90</v>
+        <v>104</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="C7" s="1"/>
     </row>
@@ -1340,48 +1348,48 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>113</v>
+        <v>127</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>116</v>
+        <v>130</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>117</v>
+        <v>131</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" ht="19">
       <c r="A5" s="2" t="s">
-        <v>90</v>
+        <v>104</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="C5" s="1"/>
     </row>
@@ -1432,30 +1440,30 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>98</v>
+        <v>112</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="C3" s="1"/>
     </row>
@@ -1516,57 +1524,57 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>122</v>
+        <v>136</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>118</v>
+        <v>132</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>105</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" ht="19">
       <c r="A5" s="2" t="s">
-        <v>120</v>
+        <v>134</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>123</v>
+        <v>0</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" ht="19">
       <c r="A6" s="2" t="s">
-        <v>121</v>
+        <v>135</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>124</v>
+        <v>1</v>
       </c>
       <c r="C6" s="1"/>
     </row>
@@ -1612,39 +1620,39 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>122</v>
+        <v>136</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>125</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>126</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c r="C4" s="1"/>
     </row>
@@ -1700,66 +1708,66 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>122</v>
+        <v>136</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>127</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>87</v>
+        <v>101</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>128</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" ht="19">
       <c r="A5" s="2" t="s">
-        <v>129</v>
+        <v>6</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" ht="19">
       <c r="A6" s="2" t="s">
-        <v>130</v>
+        <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" ht="19">
       <c r="A7" s="2" t="s">
-        <v>131</v>
+        <v>8</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="C7" s="1"/>
     </row>
@@ -1800,57 +1808,57 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>122</v>
+        <v>136</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>132</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>133</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" ht="19">
       <c r="A5" s="2" t="s">
-        <v>134</v>
+        <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" ht="19">
       <c r="A6" s="2" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="C6" s="1"/>
     </row>
@@ -1896,30 +1904,30 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="C3" s="1"/>
     </row>
@@ -1980,84 +1988,84 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" ht="19">
       <c r="A5" s="2" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" ht="19">
       <c r="A6" s="2" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" ht="19">
       <c r="A7" s="2" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" ht="19">
       <c r="A8" s="2" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>58</v>
+        <v>72</v>
       </c>
       <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:3" ht="19">
       <c r="A9" s="2" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="C9" s="1"/>
     </row>
@@ -2078,7 +2086,9 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView view="pageLayout" workbookViewId="0"/>
+    <sheetView view="pageLayout" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="17"/>
   <cols>
@@ -2088,59 +2098,67 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>122</v>
+        <v>136</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" ht="19">
       <c r="A5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>7</v>
+        <v>21</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>71</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" ht="19">
-      <c r="A6" s="2"/>
-      <c r="B6" s="1"/>
+      <c r="A6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>71</v>
+      </c>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" ht="19">
-      <c r="A7" s="2"/>
-      <c r="B7" s="1"/>
+      <c r="A7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" ht="19">
@@ -2180,30 +2198,30 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>122</v>
+        <v>136</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>105</v>
       </c>
       <c r="C3" s="1"/>
     </row>
@@ -2264,57 +2282,57 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>122</v>
+        <v>136</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" ht="19">
       <c r="A5" s="2" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" ht="19">
       <c r="A6" s="2" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="C6" s="1"/>
     </row>
@@ -2360,57 +2378,57 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>122</v>
+        <v>136</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>13</v>
+        <v>27</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>83</v>
+        <v>97</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" ht="19">
       <c r="A5" s="2" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>124</v>
+        <v>1</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" ht="19">
       <c r="A6" s="2" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="C6" s="1"/>
     </row>
@@ -2456,120 +2474,120 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>122</v>
+        <v>136</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" ht="19">
       <c r="A5" s="2" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" ht="19">
       <c r="A6" s="2" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" ht="19">
       <c r="A7" s="2" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" ht="19">
       <c r="A8" s="2" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:3" ht="19">
       <c r="A9" s="2" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:3" ht="19">
       <c r="A10" s="2" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:3" ht="19">
       <c r="A11" s="2" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="C11" s="1"/>
     </row>
     <row r="12" spans="1:3" ht="19">
       <c r="A12" s="2" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="C12" s="1"/>
     </row>
     <row r="13" spans="1:3" ht="19">
       <c r="A13" s="2" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="C13" s="1"/>
     </row>
@@ -2600,93 +2618,93 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>122</v>
+        <v>136</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" ht="19">
       <c r="A5" s="2" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>124</v>
+        <v>1</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" ht="19">
       <c r="A6" s="2" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" ht="19">
       <c r="A7" s="2" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" ht="19">
       <c r="A8" s="2" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:3" ht="19">
       <c r="A9" s="2" t="s">
-        <v>101</v>
+        <v>115</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:3" ht="19">
       <c r="A10" s="2" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="C10" s="1"/>
     </row>
@@ -2732,39 +2750,39 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>122</v>
+        <v>136</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>101</v>
+        <v>115</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="C4" s="1"/>
     </row>
@@ -2840,30 +2858,30 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>122</v>
+        <v>136</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="C3" s="1"/>
     </row>
@@ -2944,30 +2962,30 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>76</v>
+        <v>90</v>
       </c>
       <c r="C3" s="1"/>
     </row>
@@ -3028,30 +3046,30 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>75</v>
+        <v>89</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>76</v>
+        <v>90</v>
       </c>
       <c r="C3" s="1"/>
     </row>
@@ -3112,39 +3130,39 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="C4" s="1"/>
     </row>
@@ -3200,66 +3218,66 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>83</v>
+        <v>97</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" ht="19">
       <c r="A5" s="2" t="s">
-        <v>79</v>
+        <v>93</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" ht="19">
       <c r="A6" s="2" t="s">
-        <v>81</v>
+        <v>95</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" ht="19">
       <c r="A7" s="2" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="C7" s="1"/>
     </row>
@@ -3300,66 +3318,66 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>85</v>
+        <v>99</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>87</v>
+        <v>101</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" ht="19">
       <c r="A5" s="2" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" ht="19">
       <c r="A6" s="2" t="s">
-        <v>89</v>
+        <v>103</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>57</v>
+        <v>71</v>
       </c>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" ht="19">
       <c r="A7" s="2" t="s">
-        <v>90</v>
+        <v>104</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="C7" s="1"/>
     </row>
@@ -3400,66 +3418,66 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>91</v>
+        <v>105</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>92</v>
+        <v>106</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" ht="19">
       <c r="A5" s="2" t="s">
-        <v>93</v>
+        <v>107</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" ht="19">
       <c r="A6" s="2" t="s">
-        <v>94</v>
+        <v>108</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" ht="19">
       <c r="A7" s="2" t="s">
-        <v>95</v>
+        <v>109</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c r="C7" s="1"/>
     </row>
@@ -3501,100 +3519,100 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>59</v>
+        <v>73</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>49</v>
+        <v>63</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>97</v>
+        <v>111</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>98</v>
+        <v>112</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" ht="19">
       <c r="A5" s="2" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" ht="19">
       <c r="A6" s="2" t="s">
-        <v>100</v>
+        <v>114</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" ht="19">
       <c r="A7" s="2" t="s">
-        <v>101</v>
+        <v>115</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" ht="19">
       <c r="A8" s="2" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="19">
       <c r="A9" s="2" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="18">
       <c r="A10" s="1" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert FileMaker DB for resolving conflict
</commit_message>
<xml_diff>
--- a/dist-docs/TestDBSchemeForFMS.xlsx
+++ b/dist-docs/TestDBSchemeForFMS.xlsx
@@ -45,7 +45,57 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="137">
+  <si>
+    <t>タイムスタンプ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>テキスト</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>f_id</t>
+  </si>
+  <si>
+    <t>path</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>Q2</t>
+  </si>
+  <si>
+    <t>Q3</t>
+  </si>
+  <si>
+    <t>Q4</t>
+  </si>
+  <si>
+    <t>Q5</t>
+  </si>
+  <si>
+    <t>clientid</t>
+  </si>
+  <si>
+    <t>entity</t>
+  </si>
+  <si>
+    <t>conditions</t>
+  </si>
+  <si>
+    <t>realname</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>タイムスタンプ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>limitdt</t>
+    <phoneticPr fontId="1"/>
+  </si>
   <si>
     <t>registereddt</t>
   </si>
@@ -70,12 +120,120 @@
     <t>email</t>
   </si>
   <si>
+    <t>memo</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>user_id</t>
+  </si>
+  <si>
+    <t>group_id</t>
+  </si>
+  <si>
+    <t>dest_group_id</t>
+  </si>
+  <si>
+    <t>privname</t>
+  </si>
+  <si>
+    <t>clienthost</t>
+  </si>
+  <si>
+    <t>hash</t>
+  </si>
+  <si>
+    <t>expired</t>
+  </si>
+  <si>
+    <t>タイムスタンプ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>num1</t>
+  </si>
+  <si>
+    <t>num2</t>
+  </si>
+  <si>
+    <t>num3</t>
+  </si>
+  <si>
+    <t>dt1</t>
+  </si>
+  <si>
+    <t>dt2</t>
+  </si>
+  <si>
+    <t>dt3</t>
+  </si>
+  <si>
+    <t>vc1</t>
+  </si>
+  <si>
+    <t>vc2</t>
+  </si>
+  <si>
+    <t>vc3</t>
+  </si>
+  <si>
+    <t>text1</t>
+  </si>
+  <si>
+    <t>text2</t>
+  </si>
+  <si>
+    <t>タイムスタンプ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>タイムスタンプ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>タイムスタンプ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>テキスト</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>テキスト</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>テキスト</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>テキスト</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>dt</t>
+  </si>
+  <si>
+    <t>item</t>
+  </si>
+  <si>
+    <t>customer</t>
+  </si>
+  <si>
+    <t>item_id</t>
+  </si>
+  <si>
+    <t>customer_id</t>
+  </si>
+  <si>
+    <t>タイムスタンプ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>total</t>
     <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>unitprice_master</t>
   </si>
   <si>
     <t>計算</t>
@@ -85,128 +243,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Sum ( item::amount )</t>
-  </si>
-  <si>
-    <t>user_id</t>
-  </si>
-  <si>
-    <t>group_id</t>
-  </si>
-  <si>
-    <t>dest_group_id</t>
-  </si>
-  <si>
-    <t>privname</t>
-  </si>
-  <si>
-    <t>clienthost</t>
-  </si>
-  <si>
-    <t>hash</t>
-  </si>
-  <si>
-    <t>expired</t>
-  </si>
-  <si>
-    <t>タイムスタンプ</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>num1</t>
-  </si>
-  <si>
-    <t>num2</t>
-  </si>
-  <si>
-    <t>num3</t>
-  </si>
-  <si>
-    <t>dt1</t>
-  </si>
-  <si>
-    <t>dt2</t>
-  </si>
-  <si>
-    <t>dt3</t>
-  </si>
-  <si>
-    <t>vc1</t>
-  </si>
-  <si>
-    <t>vc2</t>
-  </si>
-  <si>
-    <t>vc3</t>
-  </si>
-  <si>
-    <t>text1</t>
-  </si>
-  <si>
-    <t>text2</t>
-  </si>
-  <si>
-    <t>タイムスタンプ</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>タイムスタンプ</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>タイムスタンプ</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>テキスト</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>テキスト</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>テキスト</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>テキスト</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>dt</t>
-  </si>
-  <si>
-    <t>item</t>
-  </si>
-  <si>
-    <t>customer</t>
-  </si>
-  <si>
-    <t>item_id</t>
-  </si>
-  <si>
-    <t>customer_id</t>
-  </si>
-  <si>
-    <t>タイムスタンプ</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>total</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>unitprice_master</t>
-  </si>
-  <si>
-    <t>計算</t>
-    <rPh sb="0" eb="2">
-      <t>ケイサン</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>qty * If( unitprice = ""; product::unitprice; unitprice )</t>
   </si>
   <si>
@@ -481,44 +517,6 @@
   <si>
     <t>id</t>
     <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>タイムスタンプ</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>テキスト</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>f_id</t>
-  </si>
-  <si>
-    <t>path</t>
-  </si>
-  <si>
-    <t>Q1</t>
-  </si>
-  <si>
-    <t>Q2</t>
-  </si>
-  <si>
-    <t>Q3</t>
-  </si>
-  <si>
-    <t>Q4</t>
-  </si>
-  <si>
-    <t>Q5</t>
-  </si>
-  <si>
-    <t>clientid</t>
-  </si>
-  <si>
-    <t>entity</t>
-  </si>
-  <si>
-    <t>conditions</t>
   </si>
 </sst>
 </file>
@@ -915,7 +913,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" workbookViewId="0"/>
   </sheetViews>
@@ -927,77 +925,85 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" ht="19">
       <c r="A5" s="2" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>65</v>
+        <v>77</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" ht="19">
       <c r="A6" s="2" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" ht="19">
       <c r="A7" s="2" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" ht="19">
       <c r="A8" s="2" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="C8" s="1"/>
+    </row>
+    <row r="9" spans="1:3" ht="19">
+      <c r="A9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
@@ -1026,84 +1032,84 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="3" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="4" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C2" s="3"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="4" t="s">
-        <v>100</v>
+        <v>112</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C3" s="3"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="4" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C4" s="3"/>
     </row>
     <row r="5" spans="1:3" ht="19">
       <c r="A5" s="4" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="C5" s="3"/>
     </row>
     <row r="6" spans="1:3" ht="19">
       <c r="A6" s="4" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="C6" s="3"/>
     </row>
     <row r="7" spans="1:3" ht="19">
       <c r="A7" s="4" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="C7" s="3"/>
     </row>
     <row r="8" spans="1:3" ht="19">
       <c r="A8" s="4" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
       <c r="C8" s="3"/>
     </row>
     <row r="9" spans="1:3" ht="19">
       <c r="A9" s="4" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="C9" s="3"/>
     </row>
@@ -1134,84 +1140,84 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" ht="19">
       <c r="A5" s="2" t="s">
-        <v>110</v>
+        <v>122</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" ht="19">
       <c r="A6" s="2" t="s">
-        <v>111</v>
+        <v>123</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" ht="19">
       <c r="A7" s="2" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" ht="19">
       <c r="A8" s="2" t="s">
-        <v>113</v>
+        <v>125</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:3" ht="19">
       <c r="A9" s="2" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="C9" s="1"/>
     </row>
@@ -1242,66 +1248,66 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>114</v>
+        <v>126</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>115</v>
+        <v>127</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" ht="19">
       <c r="A5" s="2" t="s">
-        <v>116</v>
+        <v>128</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" ht="19">
       <c r="A6" s="2" t="s">
-        <v>117</v>
+        <v>129</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" ht="19">
       <c r="A7" s="2" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="C7" s="1"/>
     </row>
@@ -1342,48 +1348,48 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>115</v>
+        <v>127</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>118</v>
+        <v>130</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>119</v>
+        <v>131</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" ht="19">
       <c r="A5" s="2" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="C5" s="1"/>
     </row>
@@ -1434,30 +1440,30 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>100</v>
+        <v>112</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="C3" s="1"/>
     </row>
@@ -1518,57 +1524,57 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>124</v>
+        <v>136</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>86</v>
+        <v>98</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>121</v>
+        <v>133</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" ht="19">
       <c r="A5" s="2" t="s">
-        <v>122</v>
+        <v>134</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>125</v>
+        <v>0</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" ht="19">
       <c r="A6" s="2" t="s">
-        <v>123</v>
+        <v>135</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>126</v>
+        <v>1</v>
       </c>
       <c r="C6" s="1"/>
     </row>
@@ -1614,39 +1620,39 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>124</v>
+        <v>136</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>127</v>
+        <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>128</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="C4" s="1"/>
     </row>
@@ -1702,66 +1708,66 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>124</v>
+        <v>136</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>129</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>130</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" ht="19">
       <c r="A5" s="2" t="s">
-        <v>131</v>
+        <v>6</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" ht="19">
       <c r="A6" s="2" t="s">
-        <v>132</v>
+        <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" ht="19">
       <c r="A7" s="2" t="s">
-        <v>133</v>
+        <v>8</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="C7" s="1"/>
     </row>
@@ -1802,57 +1808,57 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>124</v>
+        <v>136</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>134</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>135</v>
+        <v>10</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" ht="19">
       <c r="A5" s="2" t="s">
-        <v>136</v>
+        <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" ht="19">
       <c r="A6" s="2" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="C6" s="1"/>
     </row>
@@ -1898,30 +1904,30 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C3" s="1"/>
     </row>
@@ -1982,84 +1988,84 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" ht="19">
       <c r="A5" s="2" t="s">
-        <v>68</v>
+        <v>80</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" ht="19">
       <c r="A6" s="2" t="s">
-        <v>69</v>
+        <v>81</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" ht="19">
       <c r="A7" s="2" t="s">
-        <v>70</v>
+        <v>82</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" ht="19">
       <c r="A8" s="2" t="s">
-        <v>71</v>
+        <v>83</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>60</v>
+        <v>72</v>
       </c>
       <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:3" ht="19">
       <c r="A9" s="2" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C9" s="1"/>
     </row>
@@ -2080,7 +2086,9 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView view="pageLayout" workbookViewId="0"/>
+    <sheetView view="pageLayout" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="17"/>
   <cols>
@@ -2090,59 +2098,67 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>124</v>
+        <v>136</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>86</v>
+        <v>98</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" ht="19">
       <c r="A5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>7</v>
+        <v>21</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>71</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" ht="19">
-      <c r="A6" s="2"/>
-      <c r="B6" s="1"/>
+      <c r="A6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>71</v>
+      </c>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" ht="19">
-      <c r="A7" s="2"/>
-      <c r="B7" s="1"/>
+      <c r="A7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>13</v>
+      </c>
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" ht="19">
@@ -2182,30 +2198,30 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>124</v>
+        <v>136</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>121</v>
+        <v>133</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
       <c r="C3" s="1"/>
     </row>
@@ -2266,57 +2282,57 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>124</v>
+        <v>136</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" ht="19">
       <c r="A5" s="2" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" ht="19">
       <c r="A6" s="2" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="C6" s="1"/>
     </row>
@@ -2362,57 +2378,57 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>124</v>
+        <v>136</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" ht="19">
       <c r="A5" s="2" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>126</v>
+        <v>1</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" ht="19">
       <c r="A6" s="2" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="C6" s="1"/>
     </row>
@@ -2458,120 +2474,120 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>124</v>
+        <v>136</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>20</v>
+        <v>32</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" ht="19">
       <c r="A5" s="2" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" ht="19">
       <c r="A6" s="2" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" ht="19">
       <c r="A7" s="2" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" ht="19">
       <c r="A8" s="2" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
       <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:3" ht="19">
       <c r="A9" s="2" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:3" ht="19">
       <c r="A10" s="2" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
       <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:3" ht="19">
       <c r="A11" s="2" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="C11" s="1"/>
     </row>
     <row r="12" spans="1:3" ht="19">
       <c r="A12" s="2" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="C12" s="1"/>
     </row>
     <row r="13" spans="1:3" ht="19">
       <c r="A13" s="2" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="C13" s="1"/>
     </row>
@@ -2602,93 +2618,93 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>124</v>
+        <v>136</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>86</v>
+        <v>98</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" ht="19">
       <c r="A5" s="2" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>126</v>
+        <v>1</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" ht="19">
       <c r="A6" s="2" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" ht="19">
       <c r="A7" s="2" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" ht="19">
       <c r="A8" s="2" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:3" ht="19">
       <c r="A9" s="2" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:3" ht="19">
       <c r="A10" s="2" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C10" s="1"/>
     </row>
@@ -2734,39 +2750,39 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>124</v>
+        <v>136</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C4" s="1"/>
     </row>
@@ -2842,30 +2858,30 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>124</v>
+        <v>136</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="C3" s="1"/>
     </row>
@@ -2946,30 +2962,30 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="C3" s="1"/>
     </row>
@@ -3030,30 +3046,30 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="C3" s="1"/>
     </row>
@@ -3114,39 +3130,39 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C4" s="1"/>
     </row>
@@ -3202,66 +3218,66 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" ht="19">
       <c r="A5" s="2" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" ht="19">
       <c r="A6" s="2" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" ht="19">
       <c r="A7" s="2" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>86</v>
+        <v>98</v>
       </c>
       <c r="C7" s="1"/>
     </row>
@@ -3302,66 +3318,66 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" ht="19">
       <c r="A5" s="2" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" ht="19">
       <c r="A6" s="2" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" ht="19">
       <c r="A7" s="2" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="C7" s="1"/>
     </row>
@@ -3392,92 +3408,83 @@
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView view="pageLayout" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
-    </sheetView>
+    <sheetView view="pageLayout" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultRowHeight="17"/>
   <cols>
     <col min="1" max="1" width="20.83203125" customWidth="1"/>
     <col min="2" max="2" width="15.83203125" customWidth="1"/>
-    <col min="3" max="3" width="24" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" ht="19">
       <c r="A5" s="2" t="s">
-        <v>95</v>
+        <v>107</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" ht="19">
       <c r="A6" s="2" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" ht="19">
       <c r="A7" s="2" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" ht="19">
-      <c r="A8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="A8" s="2"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:3" ht="19">
       <c r="A9" s="2"/>
@@ -3512,100 +3519,100 @@
   <sheetData>
     <row r="1" spans="1:3" ht="18">
       <c r="A1" s="1" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>61</v>
+        <v>73</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>62</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="19">
       <c r="A2" s="2" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" ht="19">
       <c r="A3" s="2" t="s">
-        <v>99</v>
+        <v>111</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19">
       <c r="A4" s="2" t="s">
-        <v>100</v>
+        <v>112</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" ht="19">
       <c r="A5" s="2" t="s">
-        <v>101</v>
+        <v>113</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" ht="19">
       <c r="A6" s="2" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" ht="19">
       <c r="A7" s="2" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" ht="19">
       <c r="A8" s="2" t="s">
-        <v>49</v>
+        <v>61</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="19">
       <c r="A9" s="2" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="18">
       <c r="A10" s="1" t="s">
-        <v>52</v>
+        <v>64</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update TestDBSchemeForFMS.xlsx in "dist-docs" directory
</commit_message>
<xml_diff>
--- a/dist-docs/TestDBSchemeForFMS.xlsx
+++ b/dist-docs/TestDBSchemeForFMS.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27610"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/atsushi/Desktop/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="-20" windowWidth="21600" windowHeight="14600" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="person" sheetId="1" r:id="rId1"/>
@@ -37,7 +42,10 @@
   </sheets>
   <calcPr calcId="130406" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
@@ -45,195 +53,37 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="136">
+  <si>
+    <t>registereddt</t>
+  </si>
+  <si>
+    <t>テキスト</t>
+    <phoneticPr fontId="1"/>
+  </si>
   <si>
     <t>タイムスタンプ</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>context_id</t>
+  </si>
+  <si>
+    <t>pk</t>
+  </si>
+  <si>
+    <t>hashedpasswd</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
     <t>テキスト</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>f_id</t>
-  </si>
-  <si>
-    <t>path</t>
-  </si>
-  <si>
-    <t>Q1</t>
-  </si>
-  <si>
-    <t>Q2</t>
-  </si>
-  <si>
-    <t>Q3</t>
-  </si>
-  <si>
-    <t>Q4</t>
-  </si>
-  <si>
-    <t>Q5</t>
-  </si>
-  <si>
-    <t>clientid</t>
-  </si>
-  <si>
-    <t>entity</t>
-  </si>
-  <si>
-    <t>conditions</t>
-  </si>
-  <si>
-    <t>realname</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>タイムスタンプ</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>limitdt</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>registereddt</t>
-  </si>
-  <si>
-    <t>テキスト</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>タイムスタンプ</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>context_id</t>
-  </si>
-  <si>
-    <t>pk</t>
-  </si>
-  <si>
-    <t>hashedpasswd</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>memo</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>user_id</t>
-  </si>
-  <si>
-    <t>group_id</t>
-  </si>
-  <si>
-    <t>dest_group_id</t>
-  </si>
-  <si>
-    <t>privname</t>
-  </si>
-  <si>
-    <t>clienthost</t>
-  </si>
-  <si>
-    <t>hash</t>
-  </si>
-  <si>
-    <t>expired</t>
-  </si>
-  <si>
-    <t>タイムスタンプ</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>num1</t>
-  </si>
-  <si>
-    <t>num2</t>
-  </si>
-  <si>
-    <t>num3</t>
-  </si>
-  <si>
-    <t>dt1</t>
-  </si>
-  <si>
-    <t>dt2</t>
-  </si>
-  <si>
-    <t>dt3</t>
-  </si>
-  <si>
-    <t>vc1</t>
-  </si>
-  <si>
-    <t>vc2</t>
-  </si>
-  <si>
-    <t>vc3</t>
-  </si>
-  <si>
-    <t>text1</t>
-  </si>
-  <si>
-    <t>text2</t>
-  </si>
-  <si>
-    <t>タイムスタンプ</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>タイムスタンプ</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>タイムスタンプ</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>テキスト</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>テキスト</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>テキスト</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>テキスト</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>dt</t>
-  </si>
-  <si>
-    <t>item</t>
-  </si>
-  <si>
-    <t>customer</t>
-  </si>
-  <si>
-    <t>item_id</t>
-  </si>
-  <si>
-    <t>customer_id</t>
-  </si>
-  <si>
-    <t>タイムスタンプ</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>total</t>
     <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>unitprice_master</t>
   </si>
   <si>
     <t>計算</t>
@@ -243,6 +93,116 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>Sum ( item::amount )</t>
+  </si>
+  <si>
+    <t>user_id</t>
+  </si>
+  <si>
+    <t>group_id</t>
+  </si>
+  <si>
+    <t>dest_group_id</t>
+  </si>
+  <si>
+    <t>privname</t>
+  </si>
+  <si>
+    <t>clienthost</t>
+  </si>
+  <si>
+    <t>hash</t>
+  </si>
+  <si>
+    <t>expired</t>
+  </si>
+  <si>
+    <t>タイムスタンプ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>num1</t>
+  </si>
+  <si>
+    <t>num2</t>
+  </si>
+  <si>
+    <t>num3</t>
+  </si>
+  <si>
+    <t>dt1</t>
+  </si>
+  <si>
+    <t>dt2</t>
+  </si>
+  <si>
+    <t>dt3</t>
+  </si>
+  <si>
+    <t>vc1</t>
+  </si>
+  <si>
+    <t>vc2</t>
+  </si>
+  <si>
+    <t>vc3</t>
+  </si>
+  <si>
+    <t>text1</t>
+  </si>
+  <si>
+    <t>text2</t>
+  </si>
+  <si>
+    <t>タイムスタンプ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>タイムスタンプ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>タイムスタンプ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>テキスト</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>dt</t>
+  </si>
+  <si>
+    <t>item</t>
+  </si>
+  <si>
+    <t>customer</t>
+  </si>
+  <si>
+    <t>item_id</t>
+  </si>
+  <si>
+    <t>customer_id</t>
+  </si>
+  <si>
+    <t>タイムスタンプ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>total</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>unitprice_master</t>
+  </si>
+  <si>
+    <t>計算</t>
+    <rPh sb="0" eb="2">
+      <t>ケイサン</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>qty * If( unitprice = ""; product::unitprice; unitprice )</t>
   </si>
   <si>
@@ -518,12 +478,67 @@
     <t>id</t>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>タイムスタンプ</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>テキスト</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>f_id</t>
+  </si>
+  <si>
+    <t>path</t>
+  </si>
+  <si>
+    <t>Q1</t>
+  </si>
+  <si>
+    <t>Q2</t>
+  </si>
+  <si>
+    <t>Q3</t>
+  </si>
+  <si>
+    <t>Q4</t>
+  </si>
+  <si>
+    <t>Q5</t>
+  </si>
+  <si>
+    <t>clientid</t>
+  </si>
+  <si>
+    <t>entity</t>
+  </si>
+  <si>
+    <t>conditions</t>
+  </si>
+  <si>
+    <t>オブジェクト</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>If ( 
+    GetContainerAttribute ( Self ; "filename" )  ≠ "" ; 
+        Self ;
+        Let([
+            fileName = GetValue ( Self ; 1 ) ;
+            content = Substitute ( Self ; fileName &amp; ¶ ; "")
+        ] ;
+        Base64Decode( content ; fileName )
+    )
+)</t>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="ＭＳ Ｐゴシック"/>
@@ -577,18 +592,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -911,205 +934,197 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultRowHeight="17"/>
+  <sheetFormatPr baseColWidth="12" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="20.83203125" customWidth="1"/>
     <col min="2" max="2" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18">
+    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="19">
-      <c r="A2" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C2" s="1"/>
-    </row>
-    <row r="3" spans="1:3" ht="19">
-      <c r="A3" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C3" s="1"/>
-    </row>
-    <row r="4" spans="1:3" ht="19">
-      <c r="A4" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C4" s="1"/>
-    </row>
-    <row r="5" spans="1:3" ht="19">
-      <c r="A5" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>77</v>
-      </c>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:3" ht="19">
+    <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:3" ht="19">
+    <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>68</v>
+        <v>53</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:3" ht="19">
+    <row r="8" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>69</v>
+        <v>54</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="C8" s="1"/>
-    </row>
-    <row r="9" spans="1:3" ht="19">
-      <c r="A9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>45</v>
-      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.79000000000000015" right="0.79000000000000015" top="0.98" bottom="0.98" header="0.51" footer="0.51"/>
   <pageSetup paperSize="0" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="1" OnePage="0" WScale="0"/>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="1" OnePage="0" WScale="100"/>
     </ext>
   </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView view="pageLayout" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultRowHeight="17"/>
+  <sheetFormatPr baseColWidth="12" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="20.83203125" customWidth="1"/>
     <col min="2" max="2" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18">
+    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="19">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="C2" s="3"/>
     </row>
-    <row r="3" spans="1:3" ht="19">
+    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>112</v>
+        <v>97</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="C3" s="3"/>
     </row>
-    <row r="4" spans="1:3" ht="19">
+    <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="C4" s="3"/>
     </row>
-    <row r="5" spans="1:3" ht="19">
+    <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="C5" s="3"/>
     </row>
-    <row r="6" spans="1:3" ht="19">
+    <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>116</v>
+        <v>101</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
       <c r="C6" s="3"/>
     </row>
-    <row r="7" spans="1:3" ht="19">
+    <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="C7" s="3"/>
     </row>
-    <row r="8" spans="1:3" ht="19">
+    <row r="8" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>118</v>
+        <v>103</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
       <c r="C8" s="3"/>
     </row>
-    <row r="9" spans="1:3" ht="19">
+    <row r="9" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="C9" s="3"/>
     </row>
@@ -1118,106 +1133,106 @@
   <pageMargins left="0.79000000000000015" right="0.79000000000000015" top="0.98" bottom="0.98" header="0.51" footer="0.51"/>
   <pageSetup paperSize="0" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="1" OnePage="0" WScale="0"/>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="1" OnePage="0" WScale="100"/>
     </ext>
   </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView view="pageLayout" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultRowHeight="17"/>
+  <sheetFormatPr baseColWidth="12" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="20.83203125" customWidth="1"/>
     <col min="2" max="2" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18">
+    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="19">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:3" ht="19">
+    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:3" ht="19">
+    <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="C4" s="1"/>
-    </row>
-    <row r="5" spans="1:3" ht="19">
-      <c r="A5" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="1:3" ht="19">
-      <c r="A6" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C6" s="1"/>
-    </row>
-    <row r="7" spans="1:3" ht="19">
-      <c r="A7" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C7" s="1"/>
-    </row>
-    <row r="8" spans="1:3" ht="19">
-      <c r="A8" s="2" t="s">
-        <v>125</v>
-      </c>
       <c r="B8" s="1" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:3" ht="19">
+    <row r="9" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="C9" s="1"/>
     </row>
@@ -1226,97 +1241,97 @@
   <pageMargins left="0.79000000000000015" right="0.79000000000000015" top="0.98" bottom="0.98" header="0.51" footer="0.51"/>
   <pageSetup paperSize="0" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="1" OnePage="0" WScale="0"/>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="1" OnePage="0" WScale="100"/>
     </ext>
   </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView view="pageLayout" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultRowHeight="17"/>
+  <sheetFormatPr baseColWidth="12" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="20.83203125" customWidth="1"/>
     <col min="2" max="2" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18">
+    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="19">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>126</v>
+        <v>111</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:3" ht="19">
+    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:3" ht="19">
+    <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3" ht="19">
+    <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:3" ht="19">
+    <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>129</v>
+        <v>114</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:3" ht="19">
+    <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:3" ht="19">
+    <row r="8" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:3" ht="19">
+    <row r="9" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1326,89 +1341,89 @@
   <pageMargins left="0.79000000000000015" right="0.79000000000000015" top="0.98" bottom="0.98" header="0.51" footer="0.51"/>
   <pageSetup paperSize="0" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="1" OnePage="0" WScale="0"/>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="1" OnePage="0" WScale="100"/>
     </ext>
   </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView view="pageLayout" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultRowHeight="17"/>
+  <sheetFormatPr baseColWidth="12" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="20.83203125" customWidth="1"/>
     <col min="2" max="2" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18">
+    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="19">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>127</v>
+        <v>112</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:3" ht="19">
+    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:3" ht="19">
+    <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>131</v>
+        <v>116</v>
       </c>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3" ht="19">
+    <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:3" ht="19">
+    <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:3" ht="19">
+    <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:3" ht="19">
+    <row r="8" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:3" ht="19">
+    <row r="9" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1418,81 +1433,81 @@
   <pageMargins left="0.79000000000000015" right="0.79000000000000015" top="0.98" bottom="0.98" header="0.51" footer="0.51"/>
   <pageSetup paperSize="0" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="1" OnePage="0" WScale="0"/>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="1" OnePage="0" WScale="100"/>
     </ext>
   </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView view="pageLayout" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultRowHeight="17"/>
+  <sheetFormatPr baseColWidth="12" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="20.83203125" customWidth="1"/>
     <col min="2" max="2" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18">
+    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="19">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>112</v>
+        <v>97</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:3" ht="19">
+    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:3" ht="19">
+    <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3" ht="19">
+    <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:3" ht="19">
+    <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:3" ht="19">
+    <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:3" ht="19">
+    <row r="8" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:3" ht="19">
+    <row r="9" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1502,93 +1517,93 @@
   <pageMargins left="0.79000000000000015" right="0.79000000000000015" top="0.98" bottom="0.98" header="0.51" footer="0.51"/>
   <pageSetup paperSize="0" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="1" OnePage="0" WScale="0"/>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="1" OnePage="0" WScale="100"/>
     </ext>
   </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView view="pageLayout" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultRowHeight="17"/>
+  <sheetFormatPr baseColWidth="12" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="20.83203125" customWidth="1"/>
     <col min="2" max="2" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18">
+    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="19">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:3" ht="19">
+    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:3" ht="19">
+    <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>133</v>
+        <v>118</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="C4" s="1"/>
-    </row>
-    <row r="5" spans="1:3" ht="19">
-      <c r="A5" s="2" t="s">
-        <v>134</v>
-      </c>
       <c r="B5" s="2" t="s">
-        <v>0</v>
+        <v>122</v>
       </c>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:3" ht="19">
+    <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>135</v>
+        <v>120</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>1</v>
+        <v>123</v>
       </c>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:3" ht="19">
+    <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:3" ht="19">
+    <row r="8" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:3" ht="19">
+    <row r="9" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1598,85 +1613,85 @@
   <pageMargins left="0.79000000000000015" right="0.79000000000000015" top="0.98" bottom="0.98" header="0.51" footer="0.51"/>
   <pageSetup paperSize="0" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="1" OnePage="0" WScale="0"/>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="1" OnePage="0" WScale="100"/>
     </ext>
   </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView view="pageLayout" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultRowHeight="17"/>
+  <sheetFormatPr baseColWidth="12" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="20.83203125" customWidth="1"/>
     <col min="2" max="2" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18">
+    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="19">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:3" ht="19">
+    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>124</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:3" ht="19">
+    <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>3</v>
+        <v>125</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3" ht="19">
+    <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:3" ht="19">
+    <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:3" ht="19">
+    <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:3" ht="19">
+    <row r="8" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:3" ht="19">
+    <row r="9" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1686,97 +1701,97 @@
   <pageMargins left="0.79000000000000015" right="0.79000000000000015" top="0.98" bottom="0.98" header="0.51" footer="0.51"/>
   <pageSetup paperSize="0" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="1" OnePage="0" WScale="0"/>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="1" OnePage="0" WScale="100"/>
     </ext>
   </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView view="pageLayout" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultRowHeight="17"/>
+  <sheetFormatPr baseColWidth="12" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="20.83203125" customWidth="1"/>
     <col min="2" max="2" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18">
+    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="19">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:3" ht="19">
+    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>4</v>
+        <v>126</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:3" ht="19">
+    <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>5</v>
+        <v>127</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3" ht="19">
+    <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>6</v>
+        <v>128</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:3" ht="19">
+    <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>7</v>
+        <v>129</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:3" ht="19">
+    <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>8</v>
+        <v>130</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:3" ht="19">
+    <row r="8" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:3" ht="19">
+    <row r="9" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1786,93 +1801,93 @@
   <pageMargins left="0.79000000000000015" right="0.79000000000000015" top="0.98" bottom="0.98" header="0.51" footer="0.51"/>
   <pageSetup paperSize="0" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="1" OnePage="0" WScale="0"/>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="1" OnePage="0" WScale="100"/>
     </ext>
   </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView view="pageLayout" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultRowHeight="17"/>
+  <sheetFormatPr baseColWidth="12" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="20.83203125" customWidth="1"/>
     <col min="2" max="2" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18">
+    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="19">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:3" ht="19">
+    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>9</v>
+        <v>131</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:3" ht="19">
+    <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>10</v>
+        <v>132</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3" ht="19">
+    <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>11</v>
+        <v>133</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:3" ht="19">
+    <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:3" ht="19">
+    <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:3" ht="19">
+    <row r="8" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:3" ht="19">
+    <row r="9" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1882,81 +1897,81 @@
   <pageMargins left="0.79000000000000015" right="0.79000000000000015" top="0.98" bottom="0.98" header="0.51" footer="0.51"/>
   <pageSetup paperSize="0" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="1" OnePage="0" WScale="0"/>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="1" OnePage="0" WScale="100"/>
     </ext>
   </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView view="pageLayout" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultRowHeight="17"/>
+  <sheetFormatPr baseColWidth="12" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="20.83203125" customWidth="1"/>
     <col min="2" max="2" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18">
+    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="19">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:3" ht="19">
+    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:3" ht="19">
+    <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3" ht="19">
+    <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:3" ht="19">
+    <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:3" ht="19">
+    <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:3" ht="19">
+    <row r="8" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:3" ht="19">
+    <row r="9" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -1966,106 +1981,106 @@
   <pageMargins left="0.79000000000000015" right="0.79000000000000015" top="0.98" bottom="0.98" header="0.51" footer="0.51"/>
   <pageSetup paperSize="0" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="1" OnePage="0" WScale="0"/>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="1" OnePage="0" WScale="100"/>
     </ext>
   </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView view="pageLayout" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultRowHeight="17"/>
+  <sheetFormatPr baseColWidth="12" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="20.83203125" customWidth="1"/>
     <col min="2" max="2" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18">
+    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="19">
-      <c r="A2" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C2" s="1"/>
-    </row>
-    <row r="3" spans="1:3" ht="19">
-      <c r="A3" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C3" s="1"/>
-    </row>
-    <row r="4" spans="1:3" ht="19">
-      <c r="A4" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C4" s="1"/>
-    </row>
-    <row r="5" spans="1:3" ht="19">
-      <c r="A5" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="1:3" ht="19">
-      <c r="A6" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>88</v>
-      </c>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:3" ht="19">
+    <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>82</v>
+        <v>67</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:3" ht="19">
+    <row r="8" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:3" ht="19">
+    <row r="9" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="C9" s="1"/>
     </row>
@@ -2074,99 +2089,89 @@
   <pageMargins left="0.79000000000000015" right="0.79000000000000015" top="0.98" bottom="0.98" header="0.51" footer="0.51"/>
   <pageSetup paperSize="0" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="1" OnePage="0" WScale="0"/>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="1" OnePage="0" WScale="100"/>
     </ext>
   </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView view="pageLayout" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
+    <sheetView view="pageLayout" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultRowHeight="17"/>
+  <sheetFormatPr baseColWidth="12" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="20.83203125" customWidth="1"/>
     <col min="2" max="2" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18">
+    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="19">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:3" ht="19">
+    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:3" ht="19">
+    <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>20</v>
+        <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3" ht="19">
+    <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>71</v>
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:3" ht="19">
-      <c r="A6" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>71</v>
-      </c>
+    <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A6" s="2"/>
+      <c r="B6" s="1"/>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:3" ht="19">
-      <c r="A7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>13</v>
-      </c>
+    <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A7" s="2"/>
+      <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:3" ht="19">
+    <row r="8" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:3" ht="19">
+    <row r="9" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -2176,81 +2181,81 @@
   <pageMargins left="0.79000000000000015" right="0.79000000000000015" top="0.98" bottom="0.98" header="0.51" footer="0.51"/>
   <pageSetup paperSize="0" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="1" OnePage="0" WScale="0"/>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="1" OnePage="0" WScale="100"/>
     </ext>
   </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView view="pageLayout" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultRowHeight="17"/>
+  <sheetFormatPr baseColWidth="12" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="20.83203125" customWidth="1"/>
     <col min="2" max="2" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18">
+    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="19">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:3" ht="19">
+    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>133</v>
+        <v>118</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:3" ht="19">
+    <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3" ht="19">
+    <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:3" ht="19">
+    <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:3" ht="19">
+    <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:3" ht="19">
+    <row r="8" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:3" ht="19">
+    <row r="9" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -2260,93 +2265,93 @@
   <pageMargins left="0.79000000000000015" right="0.79000000000000015" top="0.98" bottom="0.98" header="0.51" footer="0.51"/>
   <pageSetup paperSize="0" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="1" OnePage="0" WScale="0"/>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="1" OnePage="0" WScale="100"/>
     </ext>
   </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView view="pageLayout" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultRowHeight="17"/>
+  <sheetFormatPr baseColWidth="12" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="20.83203125" customWidth="1"/>
     <col min="2" max="2" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18">
+    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="19">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:3" ht="19">
+    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:3" ht="19">
+    <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3" ht="19">
+    <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:3" ht="19">
+    <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:3" ht="19">
+    <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:3" ht="19">
+    <row r="8" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:3" ht="19">
+    <row r="9" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -2356,93 +2361,93 @@
   <pageMargins left="0.79000000000000015" right="0.79000000000000015" top="0.98" bottom="0.98" header="0.51" footer="0.51"/>
   <pageSetup paperSize="0" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="1" OnePage="0" WScale="0"/>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="1" OnePage="0" WScale="100"/>
     </ext>
   </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView view="pageLayout" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultRowHeight="17"/>
+  <sheetFormatPr baseColWidth="12" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="20.83203125" customWidth="1"/>
     <col min="2" max="2" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18">
+    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="19">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:3" ht="19">
+    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:3" ht="19">
+    <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>97</v>
+        <v>82</v>
       </c>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3" ht="19">
+    <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>1</v>
+        <v>123</v>
       </c>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:3" ht="19">
+    <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:3" ht="19">
+    <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:3" ht="19">
+    <row r="8" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:3" ht="19">
+    <row r="9" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -2452,142 +2457,149 @@
   <pageMargins left="0.79000000000000015" right="0.79000000000000015" top="0.98" bottom="0.98" header="0.51" footer="0.51"/>
   <pageSetup paperSize="0" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="1" OnePage="0" WScale="0"/>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="1" OnePage="0" WScale="100"/>
     </ext>
   </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView view="pageLayout" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultRowHeight="17"/>
+  <sheetFormatPr baseColWidth="12" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="20.83203125" customWidth="1"/>
     <col min="2" max="2" width="15.83203125" customWidth="1"/>
+    <col min="3" max="3" width="51.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18">
+    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="19">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:3" ht="19">
+    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C3" s="1"/>
-    </row>
-    <row r="4" spans="1:3" ht="19">
-      <c r="A4" s="2" t="s">
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C4" s="1"/>
-    </row>
-    <row r="5" spans="1:3" ht="19">
-      <c r="A5" s="2" t="s">
+      <c r="C8" s="1"/>
+    </row>
+    <row r="9" spans="1:3" ht="173" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="170" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="170" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="1:3" ht="19">
-      <c r="A6" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C6" s="1"/>
-    </row>
-    <row r="7" spans="1:3" ht="19">
-      <c r="A7" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C7" s="1"/>
-    </row>
-    <row r="8" spans="1:3" ht="19">
-      <c r="A8" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C8" s="1"/>
-    </row>
-    <row r="9" spans="1:3" ht="19">
-      <c r="A9" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C9" s="1"/>
-    </row>
-    <row r="10" spans="1:3" ht="19">
-      <c r="A10" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C10" s="1"/>
-    </row>
-    <row r="11" spans="1:3" ht="19">
-      <c r="A11" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C11" s="1"/>
-    </row>
-    <row r="12" spans="1:3" ht="19">
-      <c r="A12" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:3" ht="19">
+    <row r="13" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="C13" s="1"/>
     </row>
@@ -2596,129 +2608,129 @@
   <pageMargins left="0.79000000000000015" right="0.79000000000000015" top="0.98" bottom="0.98" header="0.51" footer="0.51"/>
   <pageSetup paperSize="0" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="1" OnePage="0" WScale="0"/>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="1" OnePage="0" WScale="100"/>
     </ext>
   </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView view="pageLayout" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultRowHeight="17"/>
+  <sheetFormatPr baseColWidth="12" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="20.83203125" customWidth="1"/>
     <col min="2" max="2" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18">
+    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="19">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:3" ht="19">
+    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>54</v>
+        <v>39</v>
       </c>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:3" ht="19">
+    <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3" ht="19">
+    <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>1</v>
+        <v>123</v>
       </c>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:3" ht="19">
+    <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:3" ht="19">
+    <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:3" ht="19">
+    <row r="8" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:3" ht="19">
+    <row r="9" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:3" ht="19">
+    <row r="10" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:3" ht="19">
+    <row r="11" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:3" ht="19">
+    <row r="12" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:3" ht="19">
+    <row r="13" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -2728,105 +2740,105 @@
   <pageMargins left="0.79000000000000015" right="0.79000000000000015" top="0.98" bottom="0.98" header="0.51" footer="0.51"/>
   <pageSetup paperSize="0" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="1" OnePage="0" WScale="0"/>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="1" OnePage="0" WScale="100"/>
     </ext>
   </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView view="pageLayout" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultRowHeight="17"/>
+  <sheetFormatPr baseColWidth="12" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="20.83203125" customWidth="1"/>
     <col min="2" max="2" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18">
+    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="19">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:3" ht="19">
+    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:3" ht="19">
+    <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3" ht="19">
+    <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:3" ht="19">
+    <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:3" ht="19">
+    <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:3" ht="19">
+    <row r="8" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:3" ht="19">
+    <row r="9" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:3" ht="19">
+    <row r="10" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:3" ht="19">
+    <row r="11" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:3" ht="19">
+    <row r="12" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:3" ht="19">
+    <row r="13" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -2836,101 +2848,101 @@
   <pageMargins left="0.79000000000000015" right="0.79000000000000015" top="0.98" bottom="0.98" header="0.51" footer="0.51"/>
   <pageSetup paperSize="0" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="1" OnePage="0" WScale="0"/>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="1" OnePage="0" WScale="100"/>
     </ext>
   </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView view="pageLayout" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultRowHeight="17"/>
+  <sheetFormatPr baseColWidth="12" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="20.83203125" customWidth="1"/>
     <col min="2" max="2" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18">
+    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="19">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>136</v>
+        <v>121</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:3" ht="19">
+    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:3" ht="19">
+    <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3" ht="19">
+    <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:3" ht="19">
+    <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:3" ht="19">
+    <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:3" ht="19">
+    <row r="8" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:3" ht="19">
+    <row r="9" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:3" ht="19">
+    <row r="10" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A10" s="2"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
-    <row r="11" spans="1:3" ht="19">
+    <row r="11" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" s="2"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
     </row>
-    <row r="12" spans="1:3" ht="19">
+    <row r="12" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
     </row>
-    <row r="13" spans="1:3" ht="19">
+    <row r="13" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" s="2"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -2940,81 +2952,81 @@
   <pageMargins left="0.79000000000000015" right="0.79000000000000015" top="0.98" bottom="0.98" header="0.51" footer="0.51"/>
   <pageSetup paperSize="0" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="1" OnePage="0" WScale="0"/>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="1" OnePage="0" WScale="100"/>
     </ext>
   </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView view="pageLayout" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultRowHeight="17"/>
+  <sheetFormatPr baseColWidth="12" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="20.83203125" customWidth="1"/>
     <col min="2" max="2" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18">
+    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="19">
-      <c r="A2" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C2" s="1"/>
-    </row>
-    <row r="3" spans="1:3" ht="19">
-      <c r="A3" s="2" t="s">
-        <v>89</v>
-      </c>
       <c r="B3" s="1" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:3" ht="19">
+    <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3" ht="19">
+    <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:3" ht="19">
+    <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:3" ht="19">
+    <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:3" ht="19">
+    <row r="8" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:3" ht="19">
+    <row r="9" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -3024,81 +3036,81 @@
   <pageMargins left="0.79000000000000015" right="0.79000000000000015" top="0.98" bottom="0.98" header="0.51" footer="0.51"/>
   <pageSetup paperSize="0" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="1" OnePage="0" WScale="0"/>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="1" OnePage="0" WScale="100"/>
     </ext>
   </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView view="pageLayout" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultRowHeight="17"/>
+  <sheetFormatPr baseColWidth="12" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="20.83203125" customWidth="1"/>
     <col min="2" max="2" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18">
+    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="19">
-      <c r="A2" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C2" s="1"/>
-    </row>
-    <row r="3" spans="1:3" ht="19">
-      <c r="A3" s="2" t="s">
-        <v>89</v>
-      </c>
       <c r="B3" s="1" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:3" ht="19">
+    <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3" ht="19">
+    <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:3" ht="19">
+    <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:3" ht="19">
+    <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:3" ht="19">
+    <row r="8" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:3" ht="19">
+    <row r="9" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -3108,85 +3120,85 @@
   <pageMargins left="0.79000000000000015" right="0.79000000000000015" top="0.98" bottom="0.98" header="0.51" footer="0.51"/>
   <pageSetup paperSize="0" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="1" OnePage="0" WScale="0"/>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="1" OnePage="0" WScale="100"/>
     </ext>
   </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView view="pageLayout" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultRowHeight="17"/>
+  <sheetFormatPr baseColWidth="12" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="20.83203125" customWidth="1"/>
     <col min="2" max="2" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18">
+    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="19">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:3" ht="19">
+    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:3" ht="19">
+    <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3" ht="19">
+    <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" s="2"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:3" ht="19">
+    <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A6" s="2"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:3" ht="19">
+    <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" s="2"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:3" ht="19">
+    <row r="8" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:3" ht="19">
+    <row r="9" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -3196,97 +3208,97 @@
   <pageMargins left="0.79000000000000015" right="0.79000000000000015" top="0.98" bottom="0.98" header="0.51" footer="0.51"/>
   <pageSetup paperSize="0" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="1" OnePage="0" WScale="0"/>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="1" OnePage="0" WScale="100"/>
     </ext>
   </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView view="pageLayout" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultRowHeight="17"/>
+  <sheetFormatPr baseColWidth="12" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="20.83203125" customWidth="1"/>
     <col min="2" max="2" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18">
+    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="19">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C2" s="1"/>
-    </row>
-    <row r="3" spans="1:3" ht="19">
-      <c r="A3" s="2" t="s">
+      <c r="B3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C3" s="1"/>
-    </row>
-    <row r="4" spans="1:3" ht="19">
-      <c r="A4" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C4" s="1"/>
-    </row>
-    <row r="5" spans="1:3" ht="19">
-      <c r="A5" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>94</v>
-      </c>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:3" ht="19">
+    <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:3" ht="19">
+    <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>98</v>
+        <v>83</v>
       </c>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:3" ht="19">
+    <row r="8" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:3" ht="19">
+    <row r="9" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -3296,97 +3308,97 @@
   <pageMargins left="0.79000000000000015" right="0.79000000000000015" top="0.98" bottom="0.98" header="0.51" footer="0.51"/>
   <pageSetup paperSize="0" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="1" OnePage="0" WScale="0"/>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="1" OnePage="0" WScale="100"/>
     </ext>
   </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView view="pageLayout" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultRowHeight="17"/>
+  <sheetFormatPr baseColWidth="12" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="20.83203125" customWidth="1"/>
     <col min="2" max="2" width="15.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18">
+    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="19">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:3" ht="19">
+    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:3" ht="19">
+    <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>100</v>
+        <v>85</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3" ht="19">
+    <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:3" ht="19">
+    <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:3" ht="19">
+    <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>75</v>
+        <v>60</v>
       </c>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:3" ht="19">
+    <row r="8" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" s="2"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
     </row>
-    <row r="9" spans="1:3" ht="19">
+    <row r="9" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -3396,97 +3408,106 @@
   <pageMargins left="0.79000000000000015" right="0.79000000000000015" top="0.98" bottom="0.98" header="0.51" footer="0.51"/>
   <pageSetup paperSize="0" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="1" OnePage="0" WScale="0"/>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="1" OnePage="0" WScale="100"/>
     </ext>
   </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView view="pageLayout" workbookViewId="0"/>
+    <sheetView view="pageLayout" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultRowHeight="17"/>
+  <sheetFormatPr baseColWidth="12" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="20.83203125" customWidth="1"/>
     <col min="2" max="2" width="15.83203125" customWidth="1"/>
+    <col min="3" max="3" width="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18">
+    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="19">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:3" ht="19">
+    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C3" s="1"/>
-    </row>
-    <row r="4" spans="1:3" ht="19">
-      <c r="A4" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C4" s="1"/>
-    </row>
-    <row r="5" spans="1:3" ht="19">
-      <c r="A5" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="1:3" ht="19">
-      <c r="A6" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C6" s="1"/>
-    </row>
-    <row r="7" spans="1:3" ht="19">
-      <c r="A7" s="2" t="s">
-        <v>109</v>
-      </c>
       <c r="B7" s="1" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:3" ht="19">
-      <c r="A8" s="2"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-    </row>
-    <row r="9" spans="1:3" ht="19">
+    <row r="8" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="2"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -3496,123 +3517,123 @@
   <pageMargins left="0.79000000000000015" right="0.79000000000000015" top="0.98" bottom="0.98" header="0.51" footer="0.51"/>
   <pageSetup paperSize="0" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="1" OnePage="0" WScale="0"/>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="1" OnePage="0" WScale="100"/>
     </ext>
   </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView view="pageLayout" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultRowHeight="17"/>
+  <sheetFormatPr baseColWidth="12" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="20.83203125" customWidth="1"/>
     <col min="2" max="2" width="15.83203125" customWidth="1"/>
     <col min="3" max="3" width="80.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18">
+    <row r="1" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="19">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="C2" s="1"/>
     </row>
-    <row r="3" spans="1:3" ht="19">
+    <row r="3" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="C3" s="1"/>
     </row>
-    <row r="4" spans="1:3" ht="19">
+    <row r="4" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>112</v>
+        <v>97</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:3" ht="19">
+    <row r="5" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>113</v>
+        <v>98</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="C5" s="1"/>
     </row>
-    <row r="6" spans="1:3" ht="19">
+    <row r="6" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="C6" s="1"/>
     </row>
-    <row r="7" spans="1:3" ht="19">
+    <row r="7" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="C7" s="1"/>
     </row>
-    <row r="8" spans="1:3" ht="19">
+    <row r="8" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="19">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="18">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>57</v>
+        <v>42</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -3620,8 +3641,8 @@
   <pageMargins left="0.79000000000000015" right="0.79000000000000015" top="0.98" bottom="0.98" header="0.51" footer="0.51"/>
   <pageSetup paperSize="0" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="1" OnePage="0" WScale="0"/>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="1" OnePage="0" WScale="100"/>
     </ext>
   </extLst>
 </worksheet>

</xml_diff>